<commit_message>
adding melanoma to comparison
</commit_message>
<xml_diff>
--- a/ImmuneCellAnalysis/04b_DeconvoluteBulk/SurvivalSummary.xlsx
+++ b/ImmuneCellAnalysis/04b_DeconvoluteBulk/SurvivalSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabelle/Dropbox (Partners HealthCare)/FilbinLab/data_analysis/Projects/git_repos/Pedi_Immune/ImmuneCellAnalysis/04b_DeconvoluteBulk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB15508-11CC-2A4F-90AE-40392591D0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA3585C-9A8A-B744-94E5-F93D042DEB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34000" yWindow="1420" windowWidth="27640" windowHeight="16440" xr2:uid="{B8B82C78-89B1-EE44-976D-0E47C15EB1DE}"/>
+    <workbookView xWindow="-31440" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{B8B82C78-89B1-EE44-976D-0E47C15EB1DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Myeloid</t>
   </si>
@@ -61,18 +61,6 @@
     <t>Stress_Response</t>
   </si>
   <si>
-    <t>CBTN: K27M</t>
-  </si>
-  <si>
-    <t>CBTN: WT</t>
-  </si>
-  <si>
-    <t>DFCI: HGG</t>
-  </si>
-  <si>
-    <t>TCGA: IDHmut AYA</t>
-  </si>
-  <si>
     <t>Inhibitory</t>
   </si>
   <si>
@@ -101,13 +89,52 @@
   </si>
   <si>
     <t>Cytotoxic</t>
+  </si>
+  <si>
+    <t>K27M</t>
+  </si>
+  <si>
+    <t>Midline WT</t>
+  </si>
+  <si>
+    <t>HGG</t>
+  </si>
+  <si>
+    <t>IDHmut AYA</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>CBTN</t>
+  </si>
+  <si>
+    <t>DFCI (MB)</t>
+  </si>
+  <si>
+    <t>TCGA</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Pediatric</t>
+  </si>
+  <si>
+    <t>AYA (25-40)</t>
+  </si>
+  <si>
+    <t>IDHmut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,8 +158,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +197,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB9A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -360,11 +412,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -374,15 +567,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -401,12 +585,41 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFB9A2"/>
+      <color rgb="FFFF7459"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -715,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F84E50-175C-AF4A-AAE4-2B1FF4EE9892}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,38 +939,58 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12"/>
-      <c r="C2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="23" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2">
@@ -769,12 +1002,26 @@
       <c r="E3" s="4">
         <v>0.89</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>1.2E-4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="38">
+        <v>35</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
@@ -784,12 +1031,26 @@
       <c r="E4" s="7">
         <v>0.66</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
+      <c r="I4" s="7"/>
+      <c r="J4" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="37">
+        <v>43</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5">
@@ -801,12 +1062,26 @@
       <c r="E5" s="7">
         <v>0.94</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="25" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="41">
+        <v>63</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5">
@@ -818,10 +1093,24 @@
       <c r="E6" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="25" t="s">
+      <c r="F6" s="11"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="30">
+        <v>203</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5">
@@ -833,55 +1122,67 @@
       <c r="E7" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>0.19</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>0.39</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>0.15</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <v>4.7E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="12"/>
-      <c r="C11" s="19" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="20" t="s">
         <v>8</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
-        <v>12</v>
       </c>
       <c r="C12" s="2">
         <v>0.2</v>
@@ -892,13 +1193,13 @@
       <c r="E12" s="4">
         <v>0.44</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="21">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="25" t="s">
-        <v>13</v>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="C13" s="5">
         <v>0.5</v>
@@ -909,13 +1210,13 @@
       <c r="E13" s="8">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="23">
         <v>8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="25" t="s">
-        <v>14</v>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="5">
         <v>0.14000000000000001</v>
@@ -926,13 +1227,13 @@
       <c r="E14" s="7">
         <v>0.21</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="23">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="25" t="s">
-        <v>15</v>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="5">
         <v>0.25</v>
@@ -943,13 +1244,13 @@
       <c r="E15" s="7">
         <v>0.64</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="25" t="s">
-        <v>16</v>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>12</v>
       </c>
       <c r="C16" s="5">
         <v>0.17</v>
@@ -960,13 +1261,13 @@
       <c r="E16" s="7">
         <v>0.43</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="12">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="25" t="s">
-        <v>17</v>
+      <c r="B17" s="22" t="s">
+        <v>13</v>
       </c>
       <c r="C17" s="5">
         <v>0.92</v>
@@ -977,55 +1278,55 @@
       <c r="E17" s="7">
         <v>0.43</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="12">
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="B18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="14">
         <v>0.12</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="14">
         <v>0.95</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="15">
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+    </row>
+    <row r="21" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="12"/>
-      <c r="C21" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>11</v>
+      <c r="E21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="23" t="s">
-        <v>17</v>
+      <c r="B22" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C22" s="2">
         <v>0.44</v>
@@ -1036,15 +1337,15 @@
       <c r="E22" s="4">
         <v>0.97</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="25">
         <v>0.86</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="21">
+      <c r="B23" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="18">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="D23" s="7">
@@ -1053,13 +1354,13 @@
       <c r="E23" s="7">
         <v>0.47</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="23">
         <v>4.6999999999999999E-4</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="25" t="s">
-        <v>14</v>
+      <c r="B24" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="C24" s="5">
         <v>0.19</v>
@@ -1070,13 +1371,13 @@
       <c r="E24" s="7">
         <v>0.38</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="23">
         <v>1E-4</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="25" t="s">
-        <v>20</v>
+      <c r="B25" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="C25" s="5">
         <v>0.13</v>
@@ -1087,13 +1388,13 @@
       <c r="E25" s="7">
         <v>0.92</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="12">
         <v>1.4E-2</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="25" t="s">
-        <v>18</v>
+      <c r="B26" s="22" t="s">
+        <v>14</v>
       </c>
       <c r="C26" s="5">
         <v>0.69</v>
@@ -1104,13 +1405,13 @@
       <c r="E26" s="7">
         <v>0.69</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="11">
         <v>0.85</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="25" t="s">
-        <v>21</v>
+      <c r="B27" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="C27" s="5">
         <v>0.16</v>
@@ -1121,24 +1422,24 @@
       <c r="E27" s="7">
         <v>0.72</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="11">
         <v>0.2</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="16">
+      <c r="B28" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="13">
         <v>0.63</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="14">
         <v>0.72</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="14">
         <v>0.21</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="26">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>